<commit_message>
Test Data updated now
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>UserName</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>Dec$2017</t>
-  </si>
-  <si>
-    <t>malini_vaikuntam@yahoo.co.in</t>
-  </si>
-  <si>
-    <t>Nov$2016</t>
   </si>
 </sst>
 </file>
@@ -385,7 +379,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -419,19 +413,13 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="A4" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Incorporated the Encryption Decryption feature
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -25,19 +25,19 @@
     <t>v_malini@rocketmail.com</t>
   </si>
   <si>
-    <t>Nov@$2017</t>
-  </si>
-  <si>
     <t>vaikuntam.malini@yahoo.com</t>
   </si>
   <si>
-    <t>Dec$2017</t>
-  </si>
-  <si>
     <t>malini_vaikuntam@yahoo.co.in</t>
   </si>
   <si>
-    <t>Nov@$2016</t>
+    <t>Tm92QCQyMDE3</t>
+  </si>
+  <si>
+    <t>RGVjJDIwMTc=</t>
+  </si>
+  <si>
+    <t>Tm92JDIwMTY=</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -407,20 +407,20 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
@@ -429,10 +429,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId2" display="Nov@$2017"/>
     <hyperlink ref="A3" r:id="rId3"/>
     <hyperlink ref="A4" r:id="rId4"/>
-    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId5" display="Nov@$2016"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>